<commit_message>
added new graph, updated data
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/25_11-6_pd_samples-edited.xlsx
+++ b/data/01_pd-samples/25_11-6_pd_samples-edited.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9CCEC2-DA64-AE46-97E2-F3497B4F360A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C896CA1-E930-904E-BBD1-659CBC110437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-8620" windowWidth="21600" windowHeight="18700" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
+    <workbookView xWindow="4880" yWindow="500" windowWidth="22860" windowHeight="17500" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
   </bookViews>
   <sheets>
     <sheet name="25_10-16_pd_samples-edited" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="417">
   <si>
     <t>sample_id</t>
   </si>
@@ -1227,9 +1227,6 @@
   </si>
   <si>
     <t xml:space="preserve">24MN13 </t>
-  </si>
-  <si>
-    <t>24MN14</t>
   </si>
   <si>
     <t xml:space="preserve">23342-1-I1 </t>
@@ -1814,8 +1811,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2241,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4D9535-1238-AB48-B467-419735026371}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="106" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2701,7 +2700,7 @@
       <c r="A7" t="s">
         <v>131</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -2743,7 +2742,7 @@
       <c r="O7" t="s">
         <v>305</v>
       </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="9" t="s">
         <v>392</v>
       </c>
       <c r="S7" t="s">
@@ -2755,21 +2754,21 @@
       <c r="U7" t="s">
         <v>378</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" s="7" t="s">
         <v>390</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>386</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>135</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>136</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -2811,7 +2810,7 @@
       <c r="O8" t="s">
         <v>305</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="9" t="s">
         <v>391</v>
       </c>
       <c r="S8" t="s">
@@ -2823,7 +2822,7 @@
       <c r="U8" t="s">
         <v>378</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="7" t="s">
         <v>389</v>
       </c>
       <c r="W8" s="6" t="s">
@@ -2834,7 +2833,7 @@
       <c r="A9" t="s">
         <v>139</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -2876,7 +2875,7 @@
       <c r="O9" t="s">
         <v>305</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="P9" s="9" t="s">
         <v>394</v>
       </c>
       <c r="S9" t="s">
@@ -2888,7 +2887,7 @@
       <c r="U9" t="s">
         <v>378</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="7" t="s">
         <v>393</v>
       </c>
       <c r="W9" s="6" t="s">
@@ -2899,7 +2898,7 @@
       <c r="A10" t="s">
         <v>143</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>144</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -2941,7 +2940,7 @@
       <c r="O10" t="s">
         <v>305</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="9" t="s">
         <v>394</v>
       </c>
       <c r="S10" t="s">
@@ -2953,7 +2952,7 @@
       <c r="U10" t="s">
         <v>378</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V10" s="7" t="s">
         <v>396</v>
       </c>
       <c r="W10" s="6" t="s">
@@ -2964,10 +2963,10 @@
       <c r="A11" t="s">
         <v>147</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>147</v>
       </c>
       <c r="D11" s="5">
@@ -3006,8 +3005,8 @@
       <c r="O11" t="s">
         <v>305</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>408</v>
+      <c r="P11" s="10" t="s">
+        <v>407</v>
       </c>
       <c r="S11" t="s">
         <v>379</v>
@@ -3018,8 +3017,8 @@
       <c r="U11" t="s">
         <v>378</v>
       </c>
-      <c r="V11" t="s">
-        <v>399</v>
+      <c r="V11" s="7" t="s">
+        <v>398</v>
       </c>
       <c r="W11" s="6" t="s">
         <v>386</v>
@@ -3029,7 +3028,7 @@
       <c r="A12" t="s">
         <v>126</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -3071,7 +3070,7 @@
       <c r="O12" t="s">
         <v>305</v>
       </c>
-      <c r="P12" s="7" t="s">
+      <c r="P12" s="9" t="s">
         <v>394</v>
       </c>
       <c r="S12" t="s">
@@ -3083,7 +3082,7 @@
       <c r="U12" t="s">
         <v>378</v>
       </c>
-      <c r="V12" t="s">
+      <c r="V12" s="7" t="s">
         <v>397</v>
       </c>
       <c r="W12" s="6" t="s">
@@ -3094,7 +3093,7 @@
       <c r="A13" t="s">
         <v>126</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>127</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -3136,7 +3135,7 @@
       <c r="O13" t="s">
         <v>305</v>
       </c>
-      <c r="P13" s="7" t="s">
+      <c r="P13" s="9" t="s">
         <v>394</v>
       </c>
       <c r="S13" t="s">
@@ -3148,8 +3147,8 @@
       <c r="U13" t="s">
         <v>378</v>
       </c>
-      <c r="V13" t="s">
-        <v>398</v>
+      <c r="V13" s="7" t="s">
+        <v>397</v>
       </c>
       <c r="W13" s="6" t="s">
         <v>386</v>
@@ -3202,7 +3201,7 @@
         <v>316</v>
       </c>
       <c r="P14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q14">
         <v>49.954439999999998</v>
@@ -3211,13 +3210,13 @@
         <v>14.175829999999999</v>
       </c>
       <c r="U14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="V14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="51" x14ac:dyDescent="0.2">
@@ -3267,7 +3266,7 @@
         <v>316</v>
       </c>
       <c r="P15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q15">
         <v>49.954439999999998</v>
@@ -3276,13 +3275,13 @@
         <v>14.175829999999999</v>
       </c>
       <c r="U15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="V15" t="s">
         <v>17</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -3332,7 +3331,7 @@
         <v>318</v>
       </c>
       <c r="P16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q16">
         <v>50.693460000000002</v>
@@ -3341,13 +3340,13 @@
         <v>15.84652</v>
       </c>
       <c r="U16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="V16" t="s">
         <v>24</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -3397,7 +3396,7 @@
         <v>318</v>
       </c>
       <c r="P17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q17">
         <v>50.693460000000002</v>
@@ -3406,13 +3405,13 @@
         <v>15.84652</v>
       </c>
       <c r="U17" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="V17" t="s">
         <v>30</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -3428,7 +3427,7 @@
       <c r="D18" s="5">
         <v>3545531</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
@@ -3455,14 +3454,14 @@
       <c r="M18" t="s">
         <v>298</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" t="s">
         <v>302</v>
       </c>
-      <c r="O18" s="10" t="s">
+      <c r="O18" t="s">
         <v>309</v>
       </c>
       <c r="P18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q18" s="8">
         <v>43.0274</v>
@@ -3471,10 +3470,10 @@
         <v>-90.092200000000005</v>
       </c>
       <c r="W18" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="X18" t="s">
         <v>409</v>
-      </c>
-      <c r="X18" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -3490,7 +3489,7 @@
       <c r="D19" s="5">
         <v>3545532</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="4" t="s">
         <v>204</v>
       </c>
       <c r="F19" t="s">
@@ -3517,14 +3516,14 @@
       <c r="M19" t="s">
         <v>298</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" t="s">
         <v>310</v>
       </c>
-      <c r="O19" s="10" t="s">
+      <c r="O19" t="s">
         <v>311</v>
       </c>
       <c r="P19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q19">
         <v>34.574328000000001</v>
@@ -3533,10 +3532,10 @@
         <v>-86.220834999999994</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="X19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -3552,7 +3551,7 @@
       <c r="D20" s="5">
         <v>3545533</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="4" t="s">
         <v>207</v>
       </c>
       <c r="F20" t="s">
@@ -3579,14 +3578,14 @@
       <c r="M20" t="s">
         <v>298</v>
       </c>
-      <c r="N20" s="10" t="s">
+      <c r="N20" t="s">
         <v>312</v>
       </c>
-      <c r="O20" s="10" t="s">
+      <c r="O20" t="s">
         <v>313</v>
       </c>
       <c r="P20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q20">
         <v>47.550894599999999</v>
@@ -3595,10 +3594,10 @@
         <v>-121.53941880000001</v>
       </c>
       <c r="W20" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="X20" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -3648,22 +3647,22 @@
         <v>320</v>
       </c>
       <c r="P21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="S21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="T21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="U21" t="s">
         <v>321</v>
       </c>
       <c r="V21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
@@ -3713,22 +3712,22 @@
         <v>320</v>
       </c>
       <c r="P22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="S22" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="T22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="U22" t="s">
         <v>321</v>
       </c>
       <c r="V22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="34" x14ac:dyDescent="0.2">

</xml_diff>